<commit_message>
Data gathering for Sense of Place goal, sacred places and Biodiversity Habiatats goal
</commit_message>
<xml_diff>
--- a/prep/HAB/hab_estuaries.xlsx
+++ b/prep/HAB/hab_estuaries.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
   <si>
     <t>rgn_id</t>
   </si>
@@ -24,9 +24,6 @@
     <t>rgn_name</t>
   </si>
   <si>
-    <t>area_m</t>
-  </si>
-  <si>
     <t>class_name</t>
   </si>
   <si>
@@ -49,6 +46,18 @@
   </si>
   <si>
     <t>Hawaii</t>
+  </si>
+  <si>
+    <t>area_sq_m</t>
+  </si>
+  <si>
+    <t>acres</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -387,194 +396,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
+      <c r="B2">
+        <v>2010</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
         <v>293852.2</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>D2/4046.85642</f>
+        <v>72.612460019028802</v>
+      </c>
+      <c r="F2">
+        <f>D2/1000000</f>
+        <v>0.29385220000000001</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
+      <c r="B3">
+        <v>2010</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
         <v>16289.3</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f t="shared" ref="E3:E13" si="0">D3/4046.85642</f>
+        <v>4.0251736927202373</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F13" si="1">D3/1000000</f>
+        <v>1.62893E-2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
+      <c r="B4">
+        <v>2010</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
         <v>140855</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>34.806028527199388</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0.14085500000000001</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
+      <c r="B5">
+        <v>2010</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
         <v>1846880.6</v>
       </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>456.37413545796124</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>1.8468806</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
+      <c r="B6">
+        <v>2010</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
         <v>707305</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>174.77887194228649</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.70730499999999996</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
+      <c r="B7">
+        <v>2010</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
         <v>669991.69999999995</v>
       </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>165.55855470651957</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.66999169999999997</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8">
+      <c r="B8">
+        <v>2010</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
         <v>1930389.1</v>
       </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>477.00953521844991</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1.9303891000000002</v>
+      </c>
+      <c r="G8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9">
+      <c r="B9">
+        <v>2010</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
         <v>2060190.7</v>
       </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>509.08420912052026</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>2.0601907000000002</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10">
+      <c r="B10">
+        <v>2010</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
         <v>2334948.5</v>
       </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>576.97834014086425</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>2.3349484999999999</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11">
+      <c r="B11">
+        <v>2010</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11">
         <v>48297.599999999999</v>
       </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>11.934596879026412</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>4.8297599999999996E-2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
+      <c r="B12">
+        <v>2010</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12">
         <v>973.4</v>
       </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.24053237846278716</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>9.7340000000000002E-4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13">
+      <c r="B13">
+        <v>2010</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13">
         <v>115585.9</v>
       </c>
-      <c r="D13" t="s">
-        <v>6</v>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>28.56189792866434</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.11558589999999999</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates based on the working group
</commit_message>
<xml_diff>
--- a/prep/HAB/hab_estuaries.xlsx
+++ b/prep/HAB/hab_estuaries.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2130" windowWidth="22275" windowHeight="8040"/>
+    <workbookView xWindow="2160" yWindow="2140" windowWidth="22280" windowHeight="12500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -402,9 +407,9 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>4</v>
       </c>
@@ -452,7 +457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>4</v>
       </c>
@@ -477,7 +482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>4</v>
       </c>
@@ -502,7 +507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>3</v>
       </c>
@@ -527,7 +532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>3</v>
       </c>
@@ -552,7 +557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>3</v>
       </c>
@@ -577,7 +582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>2</v>
       </c>
@@ -602,7 +607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>2</v>
       </c>
@@ -627,7 +632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>2</v>
       </c>
@@ -652,7 +657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>1</v>
       </c>
@@ -677,7 +682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>1</v>
       </c>
@@ -702,7 +707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>1</v>
       </c>
@@ -729,6 +734,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -738,9 +748,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -750,8 +765,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>